<commit_message>
Updated reports - new 1st page
</commit_message>
<xml_diff>
--- a/data/cropPricesCosts.xlsx
+++ b/data/cropPricesCosts.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\geoData\SMSexport\PPSN_code\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="R ready" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="BulkDensity" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="R ready" sheetId="2" r:id="rId2"/>
+    <sheet name="BulkDensity" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,75 +26,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="65">
-  <si>
-    <t xml:space="preserve">Manitoba 2022 Costs and Prices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SoilZone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analyzed Crop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AvgAnnualCost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crop used for price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AvgAnnualPrice DolPT; Statistics Canada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conversion Factor DolPT to DolPB; Bu/Tonne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avg Annual Price DolPB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CostKnownorEstimated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source: Provincial annual crop cost reports</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dollars per Tonne</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="67">
+  <si>
+    <t>Manitoba 2022 Costs and Prices</t>
+  </si>
+  <si>
+    <t>Prov</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>SoilZone</t>
+  </si>
+  <si>
+    <t>Analyzed Crop</t>
+  </si>
+  <si>
+    <t>AvgAnnualCost</t>
+  </si>
+  <si>
+    <t>Crop used for price</t>
+  </si>
+  <si>
+    <t>AvgAnnualPrice DolPT; Statistics Canada</t>
+  </si>
+  <si>
+    <t>Conversion Factor DolPT to DolPB; Bu/Tonne</t>
+  </si>
+  <si>
+    <t>Avg Annual Price DolPB</t>
+  </si>
+  <si>
+    <t>CostKnownorEstimated</t>
+  </si>
+  <si>
+    <t>Source: Provincial annual crop cost reports</t>
+  </si>
+  <si>
+    <t>Dollars per Tonne</t>
   </si>
   <si>
     <t xml:space="preserve">Conversion factors from Manitoba Statistics at https://www.gov.mb.ca/agriculture/markets-and-statistics/statistics-tables/pubs/crop_conversion_factors.pdf  except for lentils, from https://www.rayglen.com/crop-bushel-weights/ </t>
   </si>
   <si>
-    <t xml:space="preserve">Dollars per bushel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">some Alberta data will be estimated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manitoba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Black</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spring Wheat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non durum wheat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Known</t>
+    <t>Dollars per bushel</t>
+  </si>
+  <si>
+    <t>some Alberta data will be estimated</t>
+  </si>
+  <si>
+    <t>Manitoba</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Spring Wheat</t>
+  </si>
+  <si>
+    <t>Non durum wheat</t>
+  </si>
+  <si>
+    <t>Known</t>
   </si>
   <si>
     <t xml:space="preserve"> Barley</t>
   </si>
   <si>
-    <t xml:space="preserve">Barley</t>
+    <t>Barley</t>
   </si>
   <si>
     <t xml:space="preserve"> Canola</t>
@@ -99,16 +103,16 @@
     <t xml:space="preserve">Canola </t>
   </si>
   <si>
-    <t xml:space="preserve">Saskatchewan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oats</t>
+    <t>Saskatchewan</t>
+  </si>
+  <si>
+    <t>Oats</t>
   </si>
   <si>
     <t xml:space="preserve"> Rye</t>
   </si>
   <si>
-    <t xml:space="preserve">Hybrid fall rye</t>
+    <t>Hybrid fall rye</t>
   </si>
   <si>
     <t xml:space="preserve"> Spring Wheat</t>
@@ -117,19 +121,19 @@
     <t xml:space="preserve"> Mustard</t>
   </si>
   <si>
-    <t xml:space="preserve">Brown mustard</t>
+    <t>Brown mustard</t>
   </si>
   <si>
     <t xml:space="preserve"> Lentils</t>
   </si>
   <si>
-    <t xml:space="preserve">Lentils</t>
+    <t>Lentils</t>
   </si>
   <si>
     <t xml:space="preserve"> Peas</t>
   </si>
   <si>
-    <t xml:space="preserve">Dry Peas</t>
+    <t>Dry Peas</t>
   </si>
   <si>
     <t xml:space="preserve"> Soybeans</t>
@@ -141,22 +145,22 @@
     <t xml:space="preserve"> Flaxseed</t>
   </si>
   <si>
-    <t xml:space="preserve">Flaxseed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dark Brown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canola</t>
+    <t>Flaxseed</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Dark Brown</t>
+  </si>
+  <si>
+    <t>Canola</t>
   </si>
   <si>
     <t xml:space="preserve"> Chickpeas</t>
   </si>
   <si>
-    <t xml:space="preserve">Desi Chickpeas</t>
+    <t>Desi Chickpeas</t>
   </si>
   <si>
     <t xml:space="preserve"> Oats</t>
@@ -165,70 +169,74 @@
     <t xml:space="preserve"> Corn</t>
   </si>
   <si>
-    <t xml:space="preserve">Corn</t>
+    <t>Corn</t>
   </si>
   <si>
     <t xml:space="preserve"> Winter Wheat</t>
   </si>
   <si>
-    <t xml:space="preserve">Rye</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CropType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AvgCost_ha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CropUsed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CropPrice_t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SourceKnown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wheat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alberta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLACEHOLDER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mustard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soybeans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Winter Wheat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chickpeas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bu_t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Durum</t>
+    <t>Rye</t>
+  </si>
+  <si>
+    <t>CropType</t>
+  </si>
+  <si>
+    <t>AvgCost_ha</t>
+  </si>
+  <si>
+    <t>CropUsed</t>
+  </si>
+  <si>
+    <t>CropPrice_t</t>
+  </si>
+  <si>
+    <t>SourceKnown</t>
+  </si>
+  <si>
+    <t>Wheat</t>
+  </si>
+  <si>
+    <t>Alberta</t>
+  </si>
+  <si>
+    <t>PLACEHOLDER</t>
+  </si>
+  <si>
+    <t>Peas</t>
+  </si>
+  <si>
+    <t>Mustard</t>
+  </si>
+  <si>
+    <t>Soybeans</t>
+  </si>
+  <si>
+    <t>Winter Wheat</t>
+  </si>
+  <si>
+    <t>Chickpeas</t>
+  </si>
+  <si>
+    <t>Bu_t</t>
+  </si>
+  <si>
+    <t>Durum</t>
+  </si>
+  <si>
+    <t>Canaryseed</t>
+  </si>
+  <si>
+    <t>Fababeans</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="_-\$* #,##0.00_-;&quot;-$&quot;* #,##0.00_-;_-\$* \-??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.00"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-\$* #,##0.00_-;&quot;-$&quot;* #,##0.00_-;_-\$* \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -237,22 +245,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -281,7 +281,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -289,119 +289,55 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -460,40 +396,314 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="1" width="8.71"/>
+    <col min="1" max="4" width="8.7109375" style="1"/>
+    <col min="5" max="5" width="14.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="1"/>
+    <col min="10" max="10" width="17.140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -525,7 +735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="123" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="6" t="s">
         <v>11</v>
       </c>
@@ -542,11 +752,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="7" t="n">
+      <c r="B5" s="7">
         <v>2022</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -555,31 +765,31 @@
       <c r="D5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="1">
         <v>240.4</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="9" t="n">
+      <c r="G5" s="9">
         <v>446.2</v>
       </c>
-      <c r="H5" s="8" t="n">
-        <v>36.7</v>
-      </c>
-      <c r="I5" s="10" t="n">
-        <f aca="false">G5*(1/H5)</f>
-        <v>12.158038147139</v>
+      <c r="H5" s="8">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="I5" s="10">
+        <f t="shared" ref="I5:I35" si="0">G5*(1/H5)</f>
+        <v>12.158038147138962</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="7" t="n">
+      <c r="B6" s="7">
         <v>2022</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -588,31 +798,31 @@
       <c r="D6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="1">
         <v>224.44</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="9" t="n">
+      <c r="G6" s="9">
         <v>362.9</v>
       </c>
-      <c r="H6" s="1" t="n">
+      <c r="H6" s="1">
         <v>45.9</v>
       </c>
-      <c r="I6" s="10" t="n">
-        <f aca="false">G6*(1/H6)</f>
-        <v>7.90631808278867</v>
+      <c r="I6" s="10">
+        <f t="shared" si="0"/>
+        <v>7.9063180827886708</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="7" t="n">
+      <c r="B7" s="7">
         <v>2022</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -621,31 +831,31 @@
       <c r="D7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="1">
         <v>273.06</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="9" t="n">
+      <c r="G7" s="9">
         <v>959.5</v>
       </c>
-      <c r="H7" s="1" t="n">
+      <c r="H7" s="1">
         <v>44.1</v>
       </c>
-      <c r="I7" s="10" t="n">
-        <f aca="false">G7*(1/H7)</f>
-        <v>21.7573696145125</v>
+      <c r="I7" s="10">
+        <f t="shared" si="0"/>
+        <v>21.75736961451247</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="11" t="n">
+      <c r="B8" s="11">
         <v>2022</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -654,31 +864,31 @@
       <c r="D8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="11" t="n">
+      <c r="E8" s="11">
         <v>352.45</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="9" t="n">
+      <c r="G8" s="9">
         <v>484.4</v>
       </c>
-      <c r="H8" s="12" t="n">
+      <c r="H8" s="12">
         <v>64.8</v>
       </c>
-      <c r="I8" s="10" t="n">
-        <f aca="false">G8*(1/H8)</f>
-        <v>7.47530864197531</v>
+      <c r="I8" s="10">
+        <f t="shared" si="0"/>
+        <v>7.4753086419753085</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="11" t="n">
+      <c r="B9" s="11">
         <v>2022</v>
       </c>
       <c r="C9" s="11" t="s">
@@ -687,31 +897,31 @@
       <c r="D9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="11" t="n">
+      <c r="E9" s="11">
         <v>459.87</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="9" t="n">
+      <c r="G9" s="9">
         <v>952.3</v>
       </c>
-      <c r="H9" s="11" t="n">
+      <c r="H9" s="11">
         <v>44.1</v>
       </c>
-      <c r="I9" s="10" t="n">
-        <f aca="false">G9*(1/H9)</f>
-        <v>21.59410430839</v>
+      <c r="I9" s="10">
+        <f t="shared" si="0"/>
+        <v>21.594104308390023</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="11" t="n">
+      <c r="B10" s="11">
         <v>2022</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -720,31 +930,31 @@
       <c r="D10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="11" t="n">
+      <c r="E10" s="11">
         <v>342.67</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="9" t="n">
+      <c r="G10" s="9">
         <v>371.3</v>
       </c>
-      <c r="H10" s="11" t="n">
+      <c r="H10" s="11">
         <v>45.9</v>
       </c>
-      <c r="I10" s="10" t="n">
-        <f aca="false">G10*(1/H10)</f>
-        <v>8.08932461873638</v>
+      <c r="I10" s="10">
+        <f t="shared" si="0"/>
+        <v>8.0893246187363843</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="11" t="n">
+      <c r="B11" s="11">
         <v>2022</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -753,31 +963,31 @@
       <c r="D11" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="11" t="n">
+      <c r="E11" s="11">
         <v>304.37</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="9" t="n">
+      <c r="G11" s="9">
         <v>330</v>
       </c>
-      <c r="H11" s="11" t="n">
-        <v>39.368</v>
-      </c>
-      <c r="I11" s="10" t="n">
-        <f aca="false">G11*(1/H11)</f>
-        <v>8.38244259296891</v>
+      <c r="H11" s="11">
+        <v>39.368000000000002</v>
+      </c>
+      <c r="I11" s="10">
+        <f t="shared" si="0"/>
+        <v>8.3824425929689088</v>
       </c>
       <c r="J11" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="11" t="n">
+      <c r="B12" s="11">
         <v>2022</v>
       </c>
       <c r="C12" s="11" t="s">
@@ -786,31 +996,31 @@
       <c r="D12" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="11" t="n">
+      <c r="E12" s="11">
         <v>396.15</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="9" t="n">
+      <c r="G12" s="9">
         <v>446.3</v>
       </c>
-      <c r="H12" s="11" t="n">
-        <v>36.7</v>
-      </c>
-      <c r="I12" s="10" t="n">
-        <f aca="false">G12*(1/H12)</f>
-        <v>12.1607629427793</v>
+      <c r="H12" s="11">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="I12" s="10">
+        <f t="shared" si="0"/>
+        <v>12.160762942779291</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="11" t="n">
+      <c r="B13" s="11">
         <v>2022</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -819,31 +1029,31 @@
       <c r="D13" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="11" t="n">
+      <c r="E13" s="11">
         <v>240.91</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="9" t="n">
+      <c r="G13" s="9">
         <v>2050</v>
       </c>
-      <c r="H13" s="11" t="n">
+      <c r="H13" s="11">
         <v>40</v>
       </c>
-      <c r="I13" s="10" t="n">
-        <f aca="false">G13*(1/H13)</f>
+      <c r="I13" s="10">
+        <f t="shared" si="0"/>
         <v>51.25</v>
       </c>
       <c r="J13" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="11" t="n">
+      <c r="B14" s="11">
         <v>2022</v>
       </c>
       <c r="C14" s="11" t="s">
@@ -852,31 +1062,31 @@
       <c r="D14" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="11" t="n">
-        <v>269.85</v>
+      <c r="E14" s="11">
+        <v>269.85000000000002</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="9" t="n">
+      <c r="G14" s="9">
         <v>909.9</v>
       </c>
-      <c r="H14" s="11" t="n">
-        <v>36.7</v>
-      </c>
-      <c r="I14" s="10" t="n">
-        <f aca="false">G14*(1/H14)</f>
-        <v>24.7929155313351</v>
+      <c r="H14" s="11">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="I14" s="10">
+        <f t="shared" si="0"/>
+        <v>24.792915531335147</v>
       </c>
       <c r="J14" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="11" t="n">
+      <c r="B15" s="11">
         <v>2022</v>
       </c>
       <c r="C15" s="11" t="s">
@@ -885,31 +1095,31 @@
       <c r="D15" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="11" t="n">
+      <c r="E15" s="11">
         <v>312.55</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="9" t="n">
+      <c r="G15" s="9">
         <v>541.5</v>
       </c>
-      <c r="H15" s="11" t="n">
-        <v>36.7</v>
-      </c>
-      <c r="I15" s="10" t="n">
-        <f aca="false">G15*(1/H15)</f>
-        <v>14.7547683923706</v>
+      <c r="H15" s="11">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="I15" s="10">
+        <f t="shared" si="0"/>
+        <v>14.75476839237057</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="11" t="n">
+      <c r="B16" s="11">
         <v>2022</v>
       </c>
       <c r="C16" s="11" t="s">
@@ -918,31 +1128,31 @@
       <c r="D16" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="11" t="n">
+      <c r="E16" s="11">
         <v>291.13</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="9" t="n">
-        <v>725.32656</v>
-      </c>
-      <c r="H16" s="11" t="n">
+      <c r="G16" s="9">
+        <v>725.32655999999997</v>
+      </c>
+      <c r="H16" s="11">
         <v>36.744</v>
       </c>
-      <c r="I16" s="10" t="n">
-        <f aca="false">G16*(1/H16)</f>
-        <v>19.74</v>
+      <c r="I16" s="10">
+        <f t="shared" si="0"/>
+        <v>19.739999999999998</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="11" t="n">
+      <c r="B17" s="11">
         <v>2022</v>
       </c>
       <c r="C17" s="11" t="s">
@@ -951,31 +1161,31 @@
       <c r="D17" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="11" t="n">
+      <c r="E17" s="11">
         <v>291.48</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="9" t="n">
+      <c r="G17" s="9">
         <v>1209.22</v>
       </c>
-      <c r="H17" s="11" t="n">
-        <v>39.368</v>
-      </c>
-      <c r="I17" s="10" t="n">
-        <f aca="false">G17*(1/H17)</f>
-        <v>30.7158097947572</v>
+      <c r="H17" s="11">
+        <v>39.368000000000002</v>
+      </c>
+      <c r="I17" s="10">
+        <f t="shared" si="0"/>
+        <v>30.715809794757163</v>
       </c>
       <c r="J17" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="11" t="n">
+      <c r="B18" s="11">
         <v>2022</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -984,31 +1194,31 @@
       <c r="D18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="11" t="n">
-        <v>324.65</v>
+      <c r="E18" s="11">
+        <v>324.64999999999998</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="9" t="n">
+      <c r="G18" s="9">
         <v>446.3</v>
       </c>
-      <c r="H18" s="12" t="n">
-        <v>36.7</v>
-      </c>
-      <c r="I18" s="10" t="n">
-        <f aca="false">G18*(1/H18)</f>
-        <v>12.1607629427793</v>
+      <c r="H18" s="12">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="I18" s="10">
+        <f t="shared" si="0"/>
+        <v>12.160762942779291</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="11" t="n">
+      <c r="B19" s="11">
         <v>2022</v>
       </c>
       <c r="C19" s="11" t="s">
@@ -1017,31 +1227,31 @@
       <c r="D19" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="11" t="n">
-        <v>264.84</v>
+      <c r="E19" s="11">
+        <v>264.83999999999997</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G19" s="9" t="n">
+      <c r="G19" s="9">
         <v>541.5</v>
       </c>
-      <c r="H19" s="11" t="n">
-        <v>36.7</v>
-      </c>
-      <c r="I19" s="10" t="n">
-        <f aca="false">G19*(1/H19)</f>
-        <v>14.7547683923706</v>
+      <c r="H19" s="11">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="I19" s="10">
+        <f t="shared" si="0"/>
+        <v>14.75476839237057</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="11" t="n">
+      <c r="B20" s="11">
         <v>2022</v>
       </c>
       <c r="C20" s="11" t="s">
@@ -1050,31 +1260,31 @@
       <c r="D20" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="11" t="n">
+      <c r="E20" s="11">
         <v>240.91</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="9" t="n">
+      <c r="G20" s="9">
         <v>2050</v>
       </c>
-      <c r="H20" s="11" t="n">
+      <c r="H20" s="11">
         <v>40</v>
       </c>
-      <c r="I20" s="10" t="n">
-        <f aca="false">G20*(1/H20)</f>
+      <c r="I20" s="10">
+        <f t="shared" si="0"/>
         <v>51.25</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="11" t="n">
+      <c r="B21" s="11">
         <v>2022</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -1083,31 +1293,31 @@
       <c r="D21" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="11" t="n">
+      <c r="E21" s="11">
         <v>391.91</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="9" t="n">
+      <c r="G21" s="9">
         <v>952.3</v>
       </c>
-      <c r="H21" s="11" t="n">
+      <c r="H21" s="11">
         <v>44.1</v>
       </c>
-      <c r="I21" s="10" t="n">
-        <f aca="false">G21*(1/H21)</f>
-        <v>21.59410430839</v>
+      <c r="I21" s="10">
+        <f t="shared" si="0"/>
+        <v>21.594104308390023</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="11" t="n">
+      <c r="B22" s="11">
         <v>2022</v>
       </c>
       <c r="C22" s="11" t="s">
@@ -1116,31 +1326,31 @@
       <c r="D22" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="11" t="n">
+      <c r="E22" s="11">
         <v>256.01</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G22" s="9" t="n">
+      <c r="G22" s="9">
         <v>1209.22</v>
       </c>
-      <c r="H22" s="11" t="n">
-        <v>39.368</v>
-      </c>
-      <c r="I22" s="10" t="n">
-        <f aca="false">G22*(1/H22)</f>
-        <v>30.7158097947572</v>
+      <c r="H22" s="11">
+        <v>39.368000000000002</v>
+      </c>
+      <c r="I22" s="10">
+        <f t="shared" si="0"/>
+        <v>30.715809794757163</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="11" t="n">
+      <c r="B23" s="11">
         <v>2022</v>
       </c>
       <c r="C23" s="11" t="s">
@@ -1149,31 +1359,31 @@
       <c r="D23" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="11" t="n">
+      <c r="E23" s="11">
         <v>229.05</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G23" s="9" t="n">
+      <c r="G23" s="9">
         <v>909.9</v>
       </c>
-      <c r="H23" s="11" t="n">
-        <v>36.7</v>
-      </c>
-      <c r="I23" s="10" t="n">
-        <f aca="false">G23*(1/H23)</f>
-        <v>24.7929155313351</v>
+      <c r="H23" s="11">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="I23" s="10">
+        <f t="shared" si="0"/>
+        <v>24.792915531335147</v>
       </c>
       <c r="J23" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="11" t="n">
+      <c r="B24" s="11">
         <v>2022</v>
       </c>
       <c r="C24" s="11" t="s">
@@ -1182,31 +1392,31 @@
       <c r="D24" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="11" t="n">
+      <c r="E24" s="11">
         <v>429.92</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="9" t="n">
+      <c r="G24" s="9">
         <v>952.3</v>
       </c>
-      <c r="H24" s="11" t="n">
+      <c r="H24" s="11">
         <v>44.1</v>
       </c>
-      <c r="I24" s="10" t="n">
-        <f aca="false">G24*(1/H24)</f>
-        <v>21.59410430839</v>
+      <c r="I24" s="10">
+        <f t="shared" si="0"/>
+        <v>21.594104308390023</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="11" t="n">
+      <c r="B25" s="11">
         <v>2022</v>
       </c>
       <c r="C25" s="11" t="s">
@@ -1215,31 +1425,31 @@
       <c r="D25" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E25" s="11" t="n">
+      <c r="E25" s="11">
         <v>362.44</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="9" t="n">
+      <c r="G25" s="9">
         <v>446.3</v>
       </c>
-      <c r="H25" s="12" t="n">
-        <v>36.7</v>
-      </c>
-      <c r="I25" s="10" t="n">
-        <f aca="false">G25*(1/H25)</f>
-        <v>12.1607629427793</v>
+      <c r="H25" s="12">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="I25" s="10">
+        <f t="shared" si="0"/>
+        <v>12.160762942779291</v>
       </c>
       <c r="J25" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="11" t="n">
+      <c r="B26" s="11">
         <v>2022</v>
       </c>
       <c r="C26" s="11" t="s">
@@ -1248,31 +1458,31 @@
       <c r="D26" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="11" t="n">
-        <v>290.91</v>
+      <c r="E26" s="11">
+        <v>290.91000000000003</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G26" s="9" t="n">
+      <c r="G26" s="9">
         <v>371.3</v>
       </c>
-      <c r="H26" s="11" t="n">
+      <c r="H26" s="11">
         <v>45.9</v>
       </c>
-      <c r="I26" s="10" t="n">
-        <f aca="false">G26*(1/H26)</f>
-        <v>8.08932461873638</v>
+      <c r="I26" s="10">
+        <f t="shared" si="0"/>
+        <v>8.0893246187363843</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="11" t="n">
+      <c r="B27" s="11">
         <v>2022</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -1281,31 +1491,31 @@
       <c r="D27" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="11" t="n">
+      <c r="E27" s="11">
         <v>315.56</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G27" s="9" t="n">
+      <c r="G27" s="9">
         <v>40.35</v>
       </c>
-      <c r="H27" s="11" t="n">
-        <v>33.3</v>
-      </c>
-      <c r="I27" s="10" t="n">
-        <f aca="false">G27*(1/H27)</f>
-        <v>1.21171171171171</v>
+      <c r="H27" s="11">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="I27" s="10">
+        <f t="shared" si="0"/>
+        <v>1.211711711711712</v>
       </c>
       <c r="J27" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="11" t="n">
+      <c r="B28" s="11">
         <v>2022</v>
       </c>
       <c r="C28" s="11" t="s">
@@ -1314,31 +1524,31 @@
       <c r="D28" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="11" t="n">
+      <c r="E28" s="11">
         <v>236.45</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G28" s="9" t="n">
+      <c r="G28" s="9">
         <v>909.9</v>
       </c>
-      <c r="H28" s="11" t="n">
-        <v>36.7</v>
-      </c>
-      <c r="I28" s="10" t="n">
-        <f aca="false">G28*(1/H28)</f>
-        <v>24.7929155313351</v>
+      <c r="H28" s="11">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="I28" s="10">
+        <f t="shared" si="0"/>
+        <v>24.792915531335147</v>
       </c>
       <c r="J28" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="11" t="n">
+      <c r="B29" s="11">
         <v>2022</v>
       </c>
       <c r="C29" s="11" t="s">
@@ -1347,31 +1557,31 @@
       <c r="D29" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E29" s="11" t="n">
+      <c r="E29" s="11">
         <v>240.91</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G29" s="9" t="n">
+      <c r="G29" s="9">
         <v>2050</v>
       </c>
-      <c r="H29" s="11" t="n">
+      <c r="H29" s="11">
         <v>40</v>
       </c>
-      <c r="I29" s="10" t="n">
-        <f aca="false">G29*(1/H29)</f>
+      <c r="I29" s="10">
+        <f t="shared" si="0"/>
         <v>51.25</v>
       </c>
       <c r="J29" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="11" t="n">
+      <c r="B30" s="11">
         <v>2022</v>
       </c>
       <c r="C30" s="11" t="s">
@@ -1380,31 +1590,31 @@
       <c r="D30" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="11" t="n">
+      <c r="E30" s="11">
         <v>277.45</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G30" s="9" t="n">
+      <c r="G30" s="9">
         <v>484.4</v>
       </c>
-      <c r="H30" s="12" t="n">
+      <c r="H30" s="12">
         <v>64.8</v>
       </c>
-      <c r="I30" s="10" t="n">
-        <f aca="false">G30*(1/H30)</f>
-        <v>7.47530864197531</v>
+      <c r="I30" s="10">
+        <f t="shared" si="0"/>
+        <v>7.4753086419753085</v>
       </c>
       <c r="J30" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="11" t="n">
+      <c r="B31" s="11">
         <v>2022</v>
       </c>
       <c r="C31" s="11" t="s">
@@ -1413,31 +1623,31 @@
       <c r="D31" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E31" s="11" t="n">
+      <c r="E31" s="11">
         <v>423.57</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="G31" s="9" t="n">
+      <c r="G31" s="9">
         <v>349</v>
       </c>
-      <c r="H31" s="11" t="n">
-        <v>39.368</v>
-      </c>
-      <c r="I31" s="10" t="n">
-        <f aca="false">G31*(1/H31)</f>
-        <v>8.86506807559439</v>
+      <c r="H31" s="11">
+        <v>39.368000000000002</v>
+      </c>
+      <c r="I31" s="10">
+        <f t="shared" si="0"/>
+        <v>8.865068075594392</v>
       </c>
       <c r="J31" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="11" t="n">
+      <c r="B32" s="11">
         <v>2022</v>
       </c>
       <c r="C32" s="11" t="s">
@@ -1446,31 +1656,31 @@
       <c r="D32" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E32" s="11" t="n">
-        <v>283.65</v>
+      <c r="E32" s="11">
+        <v>283.64999999999998</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G32" s="9" t="n">
+      <c r="G32" s="9">
         <v>541.5</v>
       </c>
-      <c r="H32" s="11" t="n">
-        <v>36.7</v>
-      </c>
-      <c r="I32" s="10" t="n">
-        <f aca="false">G32*(1/H32)</f>
-        <v>14.7547683923706</v>
+      <c r="H32" s="11">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="I32" s="10">
+        <f t="shared" si="0"/>
+        <v>14.75476839237057</v>
       </c>
       <c r="J32" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="11" t="n">
+      <c r="B33" s="11">
         <v>2022</v>
       </c>
       <c r="C33" s="11" t="s">
@@ -1479,31 +1689,31 @@
       <c r="D33" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E33" s="11" t="n">
-        <v>287.91</v>
+      <c r="E33" s="11">
+        <v>287.91000000000003</v>
       </c>
       <c r="F33" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G33" s="9" t="n">
+      <c r="G33" s="9">
         <v>1209.22</v>
       </c>
-      <c r="H33" s="11" t="n">
-        <v>39.368</v>
-      </c>
-      <c r="I33" s="10" t="n">
-        <f aca="false">G33*(1/H33)</f>
-        <v>30.7158097947572</v>
+      <c r="H33" s="11">
+        <v>39.368000000000002</v>
+      </c>
+      <c r="I33" s="10">
+        <f t="shared" si="0"/>
+        <v>30.715809794757163</v>
       </c>
       <c r="J33" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="11" t="n">
+      <c r="B34" s="11">
         <v>2022</v>
       </c>
       <c r="C34" s="11" t="s">
@@ -1512,31 +1722,31 @@
       <c r="D34" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E34" s="11" t="n">
+      <c r="E34" s="11">
         <v>330.3</v>
       </c>
       <c r="F34" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G34" s="9" t="n">
+      <c r="G34" s="9">
         <v>446.3</v>
       </c>
-      <c r="H34" s="12" t="n">
-        <v>36.7</v>
-      </c>
-      <c r="I34" s="10" t="n">
-        <f aca="false">G34*(1/H34)</f>
-        <v>12.1607629427793</v>
+      <c r="H34" s="12">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="I34" s="10">
+        <f t="shared" si="0"/>
+        <v>12.160762942779291</v>
       </c>
       <c r="J34" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="11" t="n">
+      <c r="B35" s="11">
         <v>2022</v>
       </c>
       <c r="C35" s="11" t="s">
@@ -1545,62 +1755,54 @@
       <c r="D35" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E35" s="11" t="n">
+      <c r="E35" s="11">
         <v>283.17</v>
       </c>
       <c r="F35" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G35" s="9" t="n">
+      <c r="G35" s="9">
         <v>330</v>
       </c>
-      <c r="H35" s="11" t="n">
-        <v>39.368</v>
-      </c>
-      <c r="I35" s="10" t="n">
-        <f aca="false">G35*(1/H35)</f>
-        <v>8.38244259296891</v>
+      <c r="H35" s="11">
+        <v>39.368000000000002</v>
+      </c>
+      <c r="I35" s="10">
+        <f t="shared" si="0"/>
+        <v>8.3824425929689088</v>
       </c>
       <c r="J35" s="11" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:XFB71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="12.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="11.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="14" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="13" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="14" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="13" width="22.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="13" width="11.53"/>
+    <col min="1" max="1" width="12.5703125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="5" style="13" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="14" style="13" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="18" style="13" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="14" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" style="13" customWidth="1"/>
+    <col min="16383" max="16384" width="11.5703125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
@@ -1626,11 +1828,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="7" t="n">
+      <c r="B2" s="7">
         <v>2022</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -1639,24 +1841,24 @@
       <c r="D2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="15" t="n">
+      <c r="E2" s="15">
         <v>240.4</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="15" t="n">
+      <c r="G2" s="15">
         <v>446.2</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="7">
         <v>2022</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -1665,24 +1867,24 @@
       <c r="D3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="15" t="n">
+      <c r="E3" s="15">
         <v>224.44</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="15" t="n">
+      <c r="G3" s="15">
         <v>362.9</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="7" t="n">
+      <c r="B4" s="7">
         <v>2022</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -1691,24 +1893,24 @@
       <c r="D4" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="15" t="n">
+      <c r="E4" s="15">
         <v>273.06</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="15" t="n">
+      <c r="G4" s="15">
         <v>959.5</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="11" t="n">
+      <c r="B5" s="11">
         <v>2022</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -1717,24 +1919,24 @@
       <c r="D5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="16" t="n">
+      <c r="E5" s="16">
         <v>352.45</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="17" t="n">
+      <c r="G5" s="17">
         <v>484.4</v>
       </c>
       <c r="H5" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="11" t="n">
+      <c r="B6" s="11">
         <v>2022</v>
       </c>
       <c r="C6" s="11" t="s">
@@ -1743,24 +1945,24 @@
       <c r="D6" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="16" t="n">
+      <c r="E6" s="16">
         <v>459.87</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="17" t="n">
+      <c r="G6" s="17">
         <v>952.3</v>
       </c>
       <c r="H6" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="11" t="n">
+      <c r="B7" s="11">
         <v>2022</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -1769,24 +1971,24 @@
       <c r="D7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="16" t="n">
+      <c r="E7" s="16">
         <v>342.67</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="17" t="n">
+      <c r="G7" s="17">
         <v>371.3</v>
       </c>
       <c r="H7" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="11" t="n">
+      <c r="B8" s="11">
         <v>2022</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -1795,24 +1997,24 @@
       <c r="D8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="16" t="n">
+      <c r="E8" s="16">
         <v>304.37</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="17" t="n">
+      <c r="G8" s="17">
         <v>330</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="11" t="n">
+      <c r="B9" s="11">
         <v>2022</v>
       </c>
       <c r="C9" s="11" t="s">
@@ -1821,24 +2023,24 @@
       <c r="D9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="16" t="n">
+      <c r="E9" s="16">
         <v>396.15</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="17" t="n">
+      <c r="G9" s="17">
         <v>446.3</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="11" t="n">
+      <c r="B10" s="11">
         <v>2022</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -1847,24 +2049,24 @@
       <c r="D10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="16" t="n">
+      <c r="E10" s="16">
         <v>240.91</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="17" t="n">
+      <c r="G10" s="17">
         <v>2050</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="11" t="n">
+      <c r="B11" s="11">
         <v>2022</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -1873,24 +2075,24 @@
       <c r="D11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="16" t="n">
-        <v>269.85</v>
+      <c r="E11" s="16">
+        <v>269.85000000000002</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="17" t="n">
+      <c r="G11" s="17">
         <v>909.9</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="11" t="n">
+      <c r="B12" s="11">
         <v>2022</v>
       </c>
       <c r="C12" s="11" t="s">
@@ -1899,24 +2101,24 @@
       <c r="D12" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="16" t="n">
+      <c r="E12" s="16">
         <v>312.55</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="17" t="n">
+      <c r="G12" s="17">
         <v>541.5</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="11" t="n">
+      <c r="B13" s="11">
         <v>2022</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -1925,24 +2127,24 @@
       <c r="D13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="16" t="n">
+      <c r="E13" s="16">
         <v>291.13</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="17" t="n">
-        <v>725.32656</v>
+      <c r="G13" s="17">
+        <v>725.32655999999997</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="11" t="n">
+      <c r="B14" s="11">
         <v>2022</v>
       </c>
       <c r="C14" s="11" t="s">
@@ -1951,24 +2153,24 @@
       <c r="D14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="16" t="n">
+      <c r="E14" s="16">
         <v>291.48</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="17" t="n">
+      <c r="G14" s="17">
         <v>1209.22</v>
       </c>
       <c r="H14" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="11" t="n">
+      <c r="B15" s="11">
         <v>2022</v>
       </c>
       <c r="C15" s="11" t="s">
@@ -1977,24 +2179,24 @@
       <c r="D15" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="16" t="n">
-        <v>324.65</v>
+      <c r="E15" s="16">
+        <v>324.64999999999998</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="17" t="n">
+      <c r="G15" s="17">
         <v>446.3</v>
       </c>
       <c r="H15" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="11" t="n">
+      <c r="B16" s="11">
         <v>2022</v>
       </c>
       <c r="C16" s="11" t="s">
@@ -2003,24 +2205,24 @@
       <c r="D16" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="16" t="n">
-        <v>264.84</v>
+      <c r="E16" s="16">
+        <v>264.83999999999997</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="17" t="n">
+      <c r="G16" s="17">
         <v>541.5</v>
       </c>
       <c r="H16" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="11" t="n">
+      <c r="B17" s="11">
         <v>2022</v>
       </c>
       <c r="C17" s="11" t="s">
@@ -2029,24 +2231,24 @@
       <c r="D17" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="16" t="n">
+      <c r="E17" s="16">
         <v>240.91</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="17" t="n">
+      <c r="G17" s="17">
         <v>2050</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="11" t="n">
+      <c r="B18" s="11">
         <v>2022</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -2055,24 +2257,24 @@
       <c r="D18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="16" t="n">
+      <c r="E18" s="16">
         <v>391.91</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="17" t="n">
+      <c r="G18" s="17">
         <v>952.3</v>
       </c>
       <c r="H18" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="11" t="n">
+      <c r="B19" s="11">
         <v>2022</v>
       </c>
       <c r="C19" s="11" t="s">
@@ -2081,24 +2283,24 @@
       <c r="D19" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="16" t="n">
+      <c r="E19" s="16">
         <v>256.01</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="17" t="n">
+      <c r="G19" s="17">
         <v>1209.22</v>
       </c>
       <c r="H19" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="11" t="n">
+      <c r="B20" s="11">
         <v>2022</v>
       </c>
       <c r="C20" s="11" t="s">
@@ -2107,24 +2309,24 @@
       <c r="D20" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="16" t="n">
+      <c r="E20" s="16">
         <v>229.05</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="17" t="n">
+      <c r="G20" s="17">
         <v>909.9</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="11" t="n">
+      <c r="B21" s="11">
         <v>2022</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -2133,24 +2335,24 @@
       <c r="D21" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="16" t="n">
+      <c r="E21" s="16">
         <v>429.92</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="17" t="n">
+      <c r="G21" s="17">
         <v>952.3</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="11" t="n">
+      <c r="B22" s="11">
         <v>2022</v>
       </c>
       <c r="C22" s="11" t="s">
@@ -2159,24 +2361,24 @@
       <c r="D22" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="16" t="n">
+      <c r="E22" s="16">
         <v>362.44</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="17" t="n">
+      <c r="G22" s="17">
         <v>446.3</v>
       </c>
       <c r="H22" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="11" t="n">
+      <c r="B23" s="11">
         <v>2022</v>
       </c>
       <c r="C23" s="11" t="s">
@@ -2185,24 +2387,24 @@
       <c r="D23" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="16" t="n">
-        <v>290.91</v>
+      <c r="E23" s="16">
+        <v>290.91000000000003</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="17" t="n">
+      <c r="G23" s="17">
         <v>371.3</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="11" t="n">
+      <c r="B24" s="11">
         <v>2022</v>
       </c>
       <c r="C24" s="11" t="s">
@@ -2211,24 +2413,24 @@
       <c r="D24" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="16" t="n">
+      <c r="E24" s="16">
         <v>315.56</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G24" s="17" t="n">
+      <c r="G24" s="17">
         <v>40.35</v>
       </c>
       <c r="H24" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="11" t="n">
+      <c r="B25" s="11">
         <v>2022</v>
       </c>
       <c r="C25" s="11" t="s">
@@ -2237,24 +2439,24 @@
       <c r="D25" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="16" t="n">
+      <c r="E25" s="16">
         <v>236.45</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="17" t="n">
+      <c r="G25" s="17">
         <v>909.9</v>
       </c>
       <c r="H25" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="11" t="n">
+      <c r="B26" s="11">
         <v>2022</v>
       </c>
       <c r="C26" s="11" t="s">
@@ -2263,24 +2465,24 @@
       <c r="D26" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="16" t="n">
+      <c r="E26" s="16">
         <v>240.91</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G26" s="17" t="n">
+      <c r="G26" s="17">
         <v>2050</v>
       </c>
       <c r="H26" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="11" t="n">
+      <c r="B27" s="11">
         <v>2022</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -2289,24 +2491,24 @@
       <c r="D27" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="16" t="n">
+      <c r="E27" s="16">
         <v>277.45</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G27" s="17" t="n">
+      <c r="G27" s="17">
         <v>484.4</v>
       </c>
       <c r="H27" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="11" t="n">
+      <c r="B28" s="11">
         <v>2022</v>
       </c>
       <c r="C28" s="11" t="s">
@@ -2315,24 +2517,24 @@
       <c r="D28" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E28" s="16" t="n">
+      <c r="E28" s="16">
         <v>423.57</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="G28" s="17" t="n">
+      <c r="G28" s="17">
         <v>349</v>
       </c>
       <c r="H28" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="11" t="n">
+      <c r="B29" s="11">
         <v>2022</v>
       </c>
       <c r="C29" s="11" t="s">
@@ -2341,24 +2543,24 @@
       <c r="D29" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E29" s="16" t="n">
-        <v>283.65</v>
+      <c r="E29" s="16">
+        <v>283.64999999999998</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G29" s="17" t="n">
+      <c r="G29" s="17">
         <v>541.5</v>
       </c>
       <c r="H29" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="11" t="n">
+      <c r="B30" s="11">
         <v>2022</v>
       </c>
       <c r="C30" s="11" t="s">
@@ -2367,24 +2569,24 @@
       <c r="D30" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="16" t="n">
-        <v>287.91</v>
+      <c r="E30" s="16">
+        <v>287.91000000000003</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G30" s="17" t="n">
+      <c r="G30" s="17">
         <v>1209.22</v>
       </c>
       <c r="H30" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="11" t="n">
+      <c r="B31" s="11">
         <v>2022</v>
       </c>
       <c r="C31" s="11" t="s">
@@ -2393,24 +2595,24 @@
       <c r="D31" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="16" t="n">
+      <c r="E31" s="16">
         <v>330.3</v>
       </c>
       <c r="F31" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G31" s="17" t="n">
+      <c r="G31" s="17">
         <v>446.3</v>
       </c>
       <c r="H31" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="11" t="n">
+      <c r="B32" s="11">
         <v>2022</v>
       </c>
       <c r="C32" s="11" t="s">
@@ -2419,24 +2621,24 @@
       <c r="D32" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="16" t="n">
+      <c r="E32" s="16">
         <v>283.17</v>
       </c>
       <c r="F32" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G32" s="17" t="n">
+      <c r="G32" s="17">
         <v>330</v>
       </c>
       <c r="H32" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="7" t="n">
+      <c r="B33" s="7">
         <v>2022</v>
       </c>
       <c r="C33" s="7" t="s">
@@ -2445,24 +2647,24 @@
       <c r="D33" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E33" s="15" t="n">
+      <c r="E33" s="15">
         <v>224.44</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G33" s="15" t="n">
+      <c r="G33" s="15">
         <v>362.9</v>
       </c>
       <c r="H33" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="7" t="n">
+      <c r="B34" s="7">
         <v>2022</v>
       </c>
       <c r="C34" s="7" t="s">
@@ -2471,24 +2673,24 @@
       <c r="D34" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="15" t="n">
+      <c r="E34" s="15">
         <v>273.06</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G34" s="15" t="n">
+      <c r="G34" s="15">
         <v>959.5</v>
       </c>
       <c r="H34" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="7" t="n">
+      <c r="B35" s="7">
         <v>2022</v>
       </c>
       <c r="C35" s="7" t="s">
@@ -2497,24 +2699,24 @@
       <c r="D35" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E35" s="15" t="n">
+      <c r="E35" s="15">
         <v>123</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G35" s="15" t="n">
+      <c r="G35" s="15">
         <v>234</v>
       </c>
       <c r="H35" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="7" t="n">
+      <c r="B36" s="7">
         <v>2022</v>
       </c>
       <c r="C36" s="7" t="s">
@@ -2523,24 +2725,24 @@
       <c r="D36" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E36" s="15" t="n">
+      <c r="E36" s="15">
         <v>123</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="G36" s="15" t="n">
+      <c r="G36" s="15">
         <v>234</v>
       </c>
       <c r="H36" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="7" t="n">
+      <c r="B37" s="7">
         <v>2022</v>
       </c>
       <c r="C37" s="7" t="s">
@@ -2549,24 +2751,24 @@
       <c r="D37" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E37" s="15" t="n">
+      <c r="E37" s="15">
         <v>240.4</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G37" s="15" t="n">
+      <c r="G37" s="15">
         <v>446.2</v>
       </c>
       <c r="H37" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="7" t="n">
+      <c r="B38" s="7">
         <v>2022</v>
       </c>
       <c r="C38" s="7" t="s">
@@ -2575,24 +2777,24 @@
       <c r="D38" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="15" t="n">
+      <c r="E38" s="15">
         <v>123</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G38" s="15" t="n">
+      <c r="G38" s="15">
         <v>234</v>
       </c>
       <c r="H38" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B39" s="7" t="n">
+      <c r="B39" s="7">
         <v>2022</v>
       </c>
       <c r="C39" s="7" t="s">
@@ -2601,24 +2803,24 @@
       <c r="D39" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E39" s="15" t="n">
+      <c r="E39" s="15">
         <v>123</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G39" s="15" t="n">
+      <c r="G39" s="15">
         <v>234</v>
       </c>
       <c r="H39" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="7" t="n">
+      <c r="B40" s="7">
         <v>2022</v>
       </c>
       <c r="C40" s="7" t="s">
@@ -2627,24 +2829,24 @@
       <c r="D40" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E40" s="15" t="n">
+      <c r="E40" s="15">
         <v>123</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G40" s="15" t="n">
+      <c r="G40" s="15">
         <v>234</v>
       </c>
       <c r="H40" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="7" t="n">
+      <c r="B41" s="7">
         <v>2022</v>
       </c>
       <c r="C41" s="7" t="s">
@@ -2653,24 +2855,24 @@
       <c r="D41" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E41" s="15" t="n">
+      <c r="E41" s="15">
         <v>123</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G41" s="15" t="n">
+      <c r="G41" s="15">
         <v>234</v>
       </c>
       <c r="H41" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B42" s="7" t="n">
+      <c r="B42" s="7">
         <v>2022</v>
       </c>
       <c r="C42" s="7" t="s">
@@ -2679,24 +2881,24 @@
       <c r="D42" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E42" s="15" t="n">
+      <c r="E42" s="15">
         <v>123</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G42" s="15" t="n">
+      <c r="G42" s="15">
         <v>234</v>
       </c>
       <c r="H42" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B43" s="7" t="n">
+      <c r="B43" s="7">
         <v>2022</v>
       </c>
       <c r="C43" s="7" t="s">
@@ -2705,24 +2907,24 @@
       <c r="D43" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E43" s="15" t="n">
+      <c r="E43" s="15">
         <v>123</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G43" s="15" t="n">
+      <c r="G43" s="15">
         <v>234</v>
       </c>
       <c r="H43" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B44" s="7" t="n">
+      <c r="B44" s="7">
         <v>2022</v>
       </c>
       <c r="C44" s="7" t="s">
@@ -2731,24 +2933,24 @@
       <c r="D44" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="15" t="n">
+      <c r="E44" s="15">
         <v>240.4</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G44" s="15" t="n">
+      <c r="G44" s="15">
         <v>446.2</v>
       </c>
       <c r="H44" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B45" s="7" t="n">
+      <c r="B45" s="7">
         <v>2022</v>
       </c>
       <c r="C45" s="7" t="s">
@@ -2757,24 +2959,24 @@
       <c r="D45" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E45" s="15" t="n">
+      <c r="E45" s="15">
         <v>123</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G45" s="15" t="n">
+      <c r="G45" s="15">
         <v>234</v>
       </c>
       <c r="H45" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B46" s="7" t="n">
+      <c r="B46" s="7">
         <v>2022</v>
       </c>
       <c r="C46" s="7" t="s">
@@ -2783,24 +2985,24 @@
       <c r="D46" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E46" s="15" t="n">
+      <c r="E46" s="15">
         <v>224.44</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G46" s="15" t="n">
+      <c r="G46" s="15">
         <v>362.9</v>
       </c>
       <c r="H46" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="7" t="n">
+      <c r="B47" s="7">
         <v>2022</v>
       </c>
       <c r="C47" s="7" t="s">
@@ -2809,24 +3011,24 @@
       <c r="D47" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E47" s="15" t="n">
+      <c r="E47" s="15">
         <v>273.06</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G47" s="15" t="n">
+      <c r="G47" s="15">
         <v>959.5</v>
       </c>
       <c r="H47" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B48" s="7" t="n">
+      <c r="B48" s="7">
         <v>2022</v>
       </c>
       <c r="C48" s="7" t="s">
@@ -2835,24 +3037,24 @@
       <c r="D48" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E48" s="15" t="n">
+      <c r="E48" s="15">
         <v>123</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G48" s="15" t="n">
+      <c r="G48" s="15">
         <v>234</v>
       </c>
       <c r="H48" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B49" s="7" t="n">
+      <c r="B49" s="7">
         <v>2022</v>
       </c>
       <c r="C49" s="7" t="s">
@@ -2861,24 +3063,24 @@
       <c r="D49" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E49" s="15" t="n">
+      <c r="E49" s="15">
         <v>123</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="G49" s="15" t="n">
+      <c r="G49" s="15">
         <v>234</v>
       </c>
       <c r="H49" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B50" s="7" t="n">
+      <c r="B50" s="7">
         <v>2022</v>
       </c>
       <c r="C50" s="7" t="s">
@@ -2887,24 +3089,24 @@
       <c r="D50" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E50" s="15" t="n">
+      <c r="E50" s="15">
         <v>240.4</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G50" s="15" t="n">
+      <c r="G50" s="15">
         <v>446.2</v>
       </c>
       <c r="H50" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="7" t="n">
+      <c r="B51" s="7">
         <v>2022</v>
       </c>
       <c r="C51" s="7" t="s">
@@ -2913,24 +3115,24 @@
       <c r="D51" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E51" s="15" t="n">
+      <c r="E51" s="15">
         <v>123</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G51" s="15" t="n">
+      <c r="G51" s="15">
         <v>234</v>
       </c>
       <c r="H51" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B52" s="7" t="n">
+      <c r="B52" s="7">
         <v>2022</v>
       </c>
       <c r="C52" s="7" t="s">
@@ -2939,24 +3141,24 @@
       <c r="D52" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E52" s="15" t="n">
+      <c r="E52" s="15">
         <v>123</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G52" s="15" t="n">
+      <c r="G52" s="15">
         <v>234</v>
       </c>
       <c r="H52" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="7" t="n">
+      <c r="B53" s="7">
         <v>2022</v>
       </c>
       <c r="C53" s="7" t="s">
@@ -2965,24 +3167,24 @@
       <c r="D53" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E53" s="15" t="n">
+      <c r="E53" s="15">
         <v>123</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G53" s="15" t="n">
+      <c r="G53" s="15">
         <v>234</v>
       </c>
       <c r="H53" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="7" t="n">
+      <c r="B54" s="7">
         <v>2022</v>
       </c>
       <c r="C54" s="7" t="s">
@@ -2991,24 +3193,24 @@
       <c r="D54" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="15" t="n">
+      <c r="E54" s="15">
         <v>123</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G54" s="15" t="n">
+      <c r="G54" s="15">
         <v>234</v>
       </c>
       <c r="H54" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B55" s="7" t="n">
+      <c r="B55" s="7">
         <v>2022</v>
       </c>
       <c r="C55" s="7" t="s">
@@ -3017,24 +3219,24 @@
       <c r="D55" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E55" s="15" t="n">
+      <c r="E55" s="15">
         <v>123</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G55" s="15" t="n">
+      <c r="G55" s="15">
         <v>234</v>
       </c>
       <c r="H55" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="7" t="n">
+      <c r="B56" s="7">
         <v>2022</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -3043,24 +3245,24 @@
       <c r="D56" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E56" s="15" t="n">
+      <c r="E56" s="15">
         <v>123</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G56" s="15" t="n">
+      <c r="G56" s="15">
         <v>234</v>
       </c>
       <c r="H56" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="7" t="n">
+      <c r="B57" s="7">
         <v>2022</v>
       </c>
       <c r="C57" s="7" t="s">
@@ -3069,24 +3271,24 @@
       <c r="D57" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E57" s="15" t="n">
+      <c r="E57" s="15">
         <v>240.4</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G57" s="15" t="n">
+      <c r="G57" s="15">
         <v>446.2</v>
       </c>
       <c r="H57" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B58" s="7" t="n">
+      <c r="B58" s="7">
         <v>2022</v>
       </c>
       <c r="C58" s="7" t="s">
@@ -3095,24 +3297,24 @@
       <c r="D58" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E58" s="15" t="n">
+      <c r="E58" s="15">
         <v>123</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G58" s="15" t="n">
+      <c r="G58" s="15">
         <v>234</v>
       </c>
       <c r="H58" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="7" t="n">
+      <c r="B59" s="7">
         <v>2022</v>
       </c>
       <c r="C59" s="7" t="s">
@@ -3121,24 +3323,24 @@
       <c r="D59" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E59" s="15" t="n">
+      <c r="E59" s="15">
         <v>224.44</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G59" s="15" t="n">
+      <c r="G59" s="15">
         <v>362.9</v>
       </c>
       <c r="H59" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B60" s="7" t="n">
+      <c r="B60" s="7">
         <v>2022</v>
       </c>
       <c r="C60" s="7" t="s">
@@ -3147,24 +3349,24 @@
       <c r="D60" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E60" s="15" t="n">
+      <c r="E60" s="15">
         <v>273.06</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G60" s="15" t="n">
+      <c r="G60" s="15">
         <v>959.5</v>
       </c>
       <c r="H60" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B61" s="7" t="n">
+      <c r="B61" s="7">
         <v>2022</v>
       </c>
       <c r="C61" s="7" t="s">
@@ -3173,24 +3375,24 @@
       <c r="D61" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E61" s="15" t="n">
+      <c r="E61" s="15">
         <v>123</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G61" s="15" t="n">
+      <c r="G61" s="15">
         <v>234</v>
       </c>
       <c r="H61" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B62" s="7" t="n">
+      <c r="B62" s="7">
         <v>2022</v>
       </c>
       <c r="C62" s="7" t="s">
@@ -3199,24 +3401,24 @@
       <c r="D62" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E62" s="15" t="n">
+      <c r="E62" s="15">
         <v>123</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="G62" s="15" t="n">
+      <c r="G62" s="15">
         <v>234</v>
       </c>
       <c r="H62" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B63" s="7" t="n">
+      <c r="B63" s="7">
         <v>2022</v>
       </c>
       <c r="C63" s="7" t="s">
@@ -3225,24 +3427,24 @@
       <c r="D63" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E63" s="15" t="n">
+      <c r="E63" s="15">
         <v>240.4</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G63" s="15" t="n">
+      <c r="G63" s="15">
         <v>446.2</v>
       </c>
       <c r="H63" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B64" s="7" t="n">
+      <c r="B64" s="7">
         <v>2022</v>
       </c>
       <c r="C64" s="7" t="s">
@@ -3251,24 +3453,24 @@
       <c r="D64" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E64" s="15" t="n">
+      <c r="E64" s="15">
         <v>123</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G64" s="15" t="n">
+      <c r="G64" s="15">
         <v>234</v>
       </c>
       <c r="H64" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B65" s="7" t="n">
+      <c r="B65" s="7">
         <v>2022</v>
       </c>
       <c r="C65" s="7" t="s">
@@ -3277,24 +3479,24 @@
       <c r="D65" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E65" s="15" t="n">
+      <c r="E65" s="15">
         <v>123</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G65" s="15" t="n">
+      <c r="G65" s="15">
         <v>234</v>
       </c>
       <c r="H65" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B66" s="7" t="n">
+      <c r="B66" s="7">
         <v>2022</v>
       </c>
       <c r="C66" s="7" t="s">
@@ -3303,24 +3505,24 @@
       <c r="D66" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E66" s="15" t="n">
+      <c r="E66" s="15">
         <v>123</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G66" s="15" t="n">
+      <c r="G66" s="15">
         <v>234</v>
       </c>
       <c r="H66" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B67" s="7" t="n">
+      <c r="B67" s="7">
         <v>2022</v>
       </c>
       <c r="C67" s="7" t="s">
@@ -3329,24 +3531,24 @@
       <c r="D67" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E67" s="15" t="n">
+      <c r="E67" s="15">
         <v>123</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G67" s="15" t="n">
+      <c r="G67" s="15">
         <v>234</v>
       </c>
       <c r="H67" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B68" s="7" t="n">
+      <c r="B68" s="7">
         <v>2022</v>
       </c>
       <c r="C68" s="7" t="s">
@@ -3355,24 +3557,24 @@
       <c r="D68" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E68" s="15" t="n">
+      <c r="E68" s="15">
         <v>123</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G68" s="15" t="n">
+      <c r="G68" s="15">
         <v>234</v>
       </c>
       <c r="H68" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B69" s="7" t="n">
+      <c r="B69" s="7">
         <v>2022</v>
       </c>
       <c r="C69" s="7" t="s">
@@ -3381,24 +3583,24 @@
       <c r="D69" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E69" s="15" t="n">
+      <c r="E69" s="15">
         <v>123</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G69" s="15" t="n">
+      <c r="G69" s="15">
         <v>234</v>
       </c>
       <c r="H69" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B70" s="7" t="n">
+      <c r="B70" s="7">
         <v>2022</v>
       </c>
       <c r="C70" s="7" t="s">
@@ -3407,24 +3609,24 @@
       <c r="D70" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E70" s="15" t="n">
+      <c r="E70" s="15">
         <v>240.4</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G70" s="15" t="n">
+      <c r="G70" s="15">
         <v>446.2</v>
       </c>
       <c r="H70" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B71" s="7" t="n">
+      <c r="B71" s="7">
         <v>2022</v>
       </c>
       <c r="C71" s="7" t="s">
@@ -3433,13 +3635,13 @@
       <c r="D71" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E71" s="15" t="n">
+      <c r="E71" s="15">
         <v>123</v>
       </c>
       <c r="F71" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G71" s="15" t="n">
+      <c r="G71" s="15">
         <v>234</v>
       </c>
       <c r="H71" s="18" t="s">
@@ -3447,30 +3649,22 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>50</v>
       </c>
@@ -3478,135 +3672,151 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="12" t="n">
+      <c r="B2" s="12">
         <v>64.8</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="17"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="8" t="n">
-        <v>44.092</v>
+      <c r="B3" s="8">
+        <v>44.091999999999999</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="17"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="11" t="n">
+      <c r="B4" s="11">
         <v>45.9</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="17"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="8" t="n">
-        <v>39.368</v>
+      <c r="B5" s="8">
+        <v>39.368000000000002</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="17"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="11" t="n">
+      <c r="B6" s="11">
         <v>36.744</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="17"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="8" t="n">
-        <v>44.092</v>
+      <c r="B7" s="8">
+        <v>44.091999999999999</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="17"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="11" t="n">
+      <c r="B8" s="11">
         <v>36.744</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="17"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="11" t="n">
+      <c r="B9" s="11">
         <v>36.744</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="17"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="11" t="n">
+      <c r="B10" s="11">
         <v>36.744</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="17"/>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="8" t="n">
-        <v>39.368</v>
+      <c r="B11" s="8">
+        <v>39.368000000000002</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="17"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="8" t="n">
+      <c r="B12" s="8">
         <v>36.744</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="8" t="n">
+      <c r="B13" s="8">
         <v>36.744</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="8" t="n">
+      <c r="B14" s="8">
         <v>36.744</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15">
+        <f>2204.62/50</f>
+        <v>44.092399999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16">
+        <v>34.819509202453993</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Converted shape files from growers
</commit_message>
<xml_diff>
--- a/data/cropPricesCosts.xlsx
+++ b/data/cropPricesCosts.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="70">
   <si>
     <t>Manitoba 2022 Costs and Prices</t>
   </si>
@@ -227,6 +227,15 @@
   </si>
   <si>
     <t>Fababeans</t>
+  </si>
+  <si>
+    <t>Blow Out</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>DryMoisture_perc</t>
   </si>
 </sst>
 </file>
@@ -293,7 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -331,6 +340,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -3656,10 +3668,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3671,6 +3683,9 @@
       <c r="B1" s="13" t="s">
         <v>63</v>
       </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -3679,7 +3694,9 @@
       <c r="B2" s="12">
         <v>64.8</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="12">
+        <v>10</v>
+      </c>
       <c r="D2" s="17"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3687,9 +3704,11 @@
         <v>42</v>
       </c>
       <c r="B3" s="8">
-        <v>44.091999999999999</v>
-      </c>
-      <c r="C3" s="12"/>
+        <v>42.4</v>
+      </c>
+      <c r="C3" s="12">
+        <v>6.6</v>
+      </c>
       <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3699,7 +3718,9 @@
       <c r="B4" s="11">
         <v>45.9</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="12">
+        <v>10</v>
+      </c>
       <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3709,7 +3730,9 @@
       <c r="B5" s="8">
         <v>39.368000000000002</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="12">
+        <v>9.6999999999999993</v>
+      </c>
       <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3719,7 +3742,9 @@
       <c r="B6" s="11">
         <v>36.744</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="19">
+        <v>9.8000000000000007</v>
+      </c>
       <c r="D6" s="17"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3727,9 +3752,11 @@
         <v>59</v>
       </c>
       <c r="B7" s="8">
-        <v>44.091999999999999</v>
-      </c>
-      <c r="C7" s="12"/>
+        <v>42.4</v>
+      </c>
+      <c r="C7" s="12">
+        <v>6.6</v>
+      </c>
       <c r="D7" s="17"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3739,7 +3766,9 @@
       <c r="B8" s="11">
         <v>36.744</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8">
+        <v>13</v>
+      </c>
       <c r="D8" s="17"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3749,7 +3778,9 @@
       <c r="B9" s="11">
         <v>36.744</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="12">
+        <v>10</v>
+      </c>
       <c r="D9" s="17"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3759,7 +3790,9 @@
       <c r="B10" s="11">
         <v>36.744</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="12">
+        <v>7</v>
+      </c>
       <c r="D10" s="17"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3769,7 +3802,9 @@
       <c r="B11" s="8">
         <v>39.368000000000002</v>
       </c>
-      <c r="C11" s="11"/>
+      <c r="C11" s="19">
+        <v>7</v>
+      </c>
       <c r="D11" s="17"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3779,6 +3814,9 @@
       <c r="B12" s="8">
         <v>36.744</v>
       </c>
+      <c r="C12" s="19">
+        <v>9.8000000000000007</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
@@ -3787,13 +3825,19 @@
       <c r="B13" s="8">
         <v>36.744</v>
       </c>
+      <c r="C13" s="19">
+        <v>9.8000000000000007</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>62</v>
       </c>
       <c r="B14" s="8">
-        <v>36.744</v>
+        <v>38.348513513513517</v>
+      </c>
+      <c r="C14">
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3804,6 +3848,9 @@
         <f>2204.62/50</f>
         <v>44.092399999999998</v>
       </c>
+      <c r="C15" s="19">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
@@ -3811,6 +3858,20 @@
       </c>
       <c r="B16">
         <v>34.819509202453993</v>
+      </c>
+      <c r="C16" s="19">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated helper functions and added crop density data
</commit_message>
<xml_diff>
--- a/data/cropPricesCosts.xlsx
+++ b/data/cropPricesCosts.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="71">
   <si>
     <t>Manitoba 2022 Costs and Prices</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>DryMoisture_perc</t>
+  </si>
+  <si>
+    <t>Sorghum</t>
   </si>
 </sst>
 </file>
@@ -3668,10 +3671,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3872,6 +3875,17 @@
       </c>
       <c r="C17" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18">
+        <v>39.359084604715676</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>